<commit_message>
Falta comprobar el final
</commit_message>
<xml_diff>
--- a/AnalisisDatos.xlsx
+++ b/AnalisisDatos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Documents\INF\4º\ADA\adap1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Estudios\UVA\4o curso 1\ADA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA42451-6DFD-448A-939C-432FE2D6C43D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835C4484-DDD8-4E20-98F7-E9AAF145C958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{C3DD8E36-B099-4B3E-878D-B4047BB6BD03}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C3DD8E36-B099-4B3E-878D-B4047BB6BD03}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,7 +135,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -678,7 +678,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1324,7 +1324,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1856,7 +1856,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2492,7 +2492,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3024,7 +3024,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3662,7 +3662,7 @@
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3742,16 +3742,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-GB"/>
@@ -4234,7 +4231,7 @@
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4773,7 +4770,7 @@
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -10653,7 +10650,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -10951,11 +10948,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62011B8E-48A5-41C4-869D-F6112BF86A8B}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
@@ -11885,141 +11882,141 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f>3*(A3^1.2)</f>
+        <f t="shared" ref="A49:A58" si="9">3*(A3^1.2)</f>
         <v>189287.20334405801</v>
       </c>
       <c r="B49">
-        <f>1.0275*(A3^1.3)</f>
+        <f t="shared" ref="B49:B58" si="10">1.0275*(A3^1.3)</f>
         <v>162847.77552537972</v>
       </c>
       <c r="C49">
-        <f>0.3533*(A3^1.4)</f>
+        <f t="shared" ref="C49:C58" si="11">0.3533*(A3^1.4)</f>
         <v>140651.26335655054</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f>3*(A4^1.2)</f>
+        <f t="shared" si="9"/>
         <v>434867.79820661678</v>
       </c>
       <c r="B50">
-        <f>1.0275*(A4^1.3)</f>
+        <f t="shared" si="10"/>
         <v>400978.25812743546</v>
       </c>
       <c r="C50">
-        <f>0.3533*(A4^1.4)</f>
+        <f t="shared" si="11"/>
         <v>371180.90931833972</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>3*(A5^1.2)</f>
+        <f t="shared" si="9"/>
         <v>707402.7770369607</v>
       </c>
       <c r="B51">
-        <f>1.0275*(A5^1.3)</f>
+        <f t="shared" si="10"/>
         <v>679265.35050157213</v>
       </c>
       <c r="C51">
-        <f>0.3533*(A5^1.4)</f>
+        <f t="shared" si="11"/>
         <v>654807.12151639897</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>3*(A6^1.2)</f>
+        <f t="shared" si="9"/>
         <v>999063.84888224653</v>
       </c>
       <c r="B52">
-        <f>1.0275*(A6^1.3)</f>
+        <f t="shared" si="10"/>
         <v>987324.28473273688</v>
       </c>
       <c r="C52">
-        <f>0.3533*(A6^1.4)</f>
+        <f t="shared" si="11"/>
         <v>979552.2923468512</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f>3*(A7^1.2)</f>
+        <f t="shared" si="9"/>
         <v>1305825.8449441856</v>
       </c>
       <c r="B53">
-        <f>1.0275*(A7^1.3)</f>
+        <f t="shared" si="10"/>
         <v>1319601.608309743</v>
       </c>
       <c r="C53">
-        <f>0.3533*(A7^1.4)</f>
+        <f t="shared" si="11"/>
         <v>1338756.6573703072</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54">
-        <f>3*(A8^1.2)</f>
+        <f t="shared" si="9"/>
         <v>1625184.8126053824</v>
       </c>
       <c r="B54">
-        <f>1.0275*(A8^1.3)</f>
+        <f t="shared" si="10"/>
         <v>1672547.4828975725</v>
       </c>
       <c r="C54">
-        <f>0.3533*(A8^1.4)</f>
+        <f t="shared" si="11"/>
         <v>1728046.353742633</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55">
-        <f>3*(A9^1.2)</f>
+        <f t="shared" si="9"/>
         <v>1955414.821699155</v>
       </c>
       <c r="B55">
-        <f>1.0275*(A9^1.3)</f>
+        <f t="shared" si="10"/>
         <v>2043663.0016654094</v>
       </c>
       <c r="C55">
-        <f>0.3533*(A9^1.4)</f>
+        <f t="shared" si="11"/>
         <v>2144277.0305309533</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56">
-        <f>3*(A10^1.2)</f>
+        <f t="shared" si="9"/>
         <v>2295245.9994960865</v>
       </c>
       <c r="B56">
-        <f>1.0275*(A10^1.3)</f>
+        <f t="shared" si="10"/>
         <v>2431077.5546169467</v>
       </c>
       <c r="C56">
-        <f>0.3533*(A10^1.4)</f>
+        <f t="shared" si="11"/>
         <v>2585053.9975347864</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57">
-        <f>3*(A11^1.2)</f>
+        <f t="shared" si="9"/>
         <v>2643700.5783746336</v>
       </c>
       <c r="B57">
-        <f>1.0275*(A11^1.3)</f>
+        <f t="shared" si="10"/>
         <v>2833329.5613246765</v>
       </c>
       <c r="C57">
-        <f>0.3533*(A11^1.4)</f>
+        <f t="shared" si="11"/>
         <v>3048478.5998804444</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58">
-        <f>3*(A12^1.2)</f>
+        <f t="shared" si="9"/>
         <v>2999999.9999999986</v>
       </c>
       <c r="B58">
-        <f>1.0275*(A12^1.3)</f>
+        <f t="shared" si="10"/>
         <v>3249240.2958230102</v>
       </c>
       <c r="C58">
-        <f>0.3533*(A12^1.4)</f>
+        <f t="shared" si="11"/>
         <v>3533000.0000000019</v>
       </c>
     </row>
@@ -12040,137 +12037,137 @@
         <v>2.7338932101996463</v>
       </c>
       <c r="B62">
-        <f>B3/(A3^1.3)</f>
+        <f t="shared" ref="B62:B71" si="12">B3/(A3^1.3)</f>
         <v>1.0883824905079968</v>
       </c>
       <c r="C62">
-        <f>B3/(A3^1.4)</f>
+        <f t="shared" ref="C62:C71" si="13">B3/(A3^1.4)</f>
         <v>0.43329287377610815</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63">
-        <f t="shared" ref="A63:A71" si="9">B4/(A4^1.2)</f>
+        <f t="shared" ref="A63:A71" si="14">B4/(A4^1.2)</f>
         <v>2.8813584385125317</v>
       </c>
       <c r="B63">
-        <f>B4/(A4^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0702723060451058</v>
       </c>
       <c r="C63">
-        <f>B4/(A4^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.39754957029173121</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2.892931815410551</v>
       </c>
       <c r="B64">
-        <f>B5/(A5^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0318725804024032</v>
       </c>
       <c r="C64">
-        <f>B5/(A5^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.36805603800074776</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>2.9655792303112425</v>
       </c>
       <c r="B65">
-        <f>B6/(A6^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0277879752291212</v>
       </c>
       <c r="C65">
-        <f>B6/(A6^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.35620296744346813</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.0196913434260773</v>
       </c>
       <c r="B66">
-        <f>B7/(A7^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0234474624730787</v>
       </c>
       <c r="C66">
-        <f>B7/(A7^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.34687144787923246</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.0662051240876189</v>
       </c>
       <c r="B67">
-        <f>B8/(A8^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0204367244888084</v>
       </c>
       <c r="C67">
-        <f>B8/(A8^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.33960255969348985</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.0840637664593835</v>
       </c>
       <c r="B68">
-        <f>B9/(A9^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.010679705174877</v>
       </c>
       <c r="C68">
-        <f>B9/(A9^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.33121022903656383</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.1815295622356889</v>
       </c>
       <c r="B69">
-        <f>B10/(A10^1.3)</f>
+        <f t="shared" si="12"/>
         <v>1.0287905450610282</v>
       </c>
       <c r="C69">
-        <f>B10/(A10^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.33267331480120371</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.1078481682866643</v>
       </c>
       <c r="B70">
-        <f>B11/(A11^1.3)</f>
+        <f t="shared" si="12"/>
         <v>0.99319732812314809</v>
       </c>
       <c r="C70">
-        <f>B11/(A11^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.31740319319871474</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="14"/>
         <v>3.1007170000000013</v>
       </c>
       <c r="B71">
-        <f>B12/(A12^1.3)</f>
+        <f t="shared" si="12"/>
         <v>0.98053280996043157</v>
       </c>
       <c r="C71">
-        <f>B12/(A12^1.4)</f>
+        <f t="shared" si="13"/>
         <v>0.31007169999999984</v>
       </c>
     </row>

</xml_diff>